<commit_message>
made changes for incremental load test scenarios
</commit_message>
<xml_diff>
--- a/Module_2/test_cases_dq_checks.xlsx
+++ b/Module_2/test_cases_dq_checks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana_kalandadze\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana_kalandadze\Desktop\DQE_int\Module_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2C55AC-6374-4D2C-97BF-E4FC6C55AD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD906FED-F9FC-40E1-A968-261052B5AEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="243">
   <si>
     <t>Source</t>
   </si>
@@ -171,16 +171,6 @@
     <t>Test the rollback mechanism to ensure that if an error occurs during the incremental update process, the data is rolled back to its previous state without corruption or loss.</t>
   </si>
   <si>
-    <t>Test the scenario where forecast rates are updated for existing combinations of store group + store_group1 + store_group2 + year_month.
-Verify that the updated forecast rates are correctly reflected in the target table.
-Ensure that only the affected rows are updated, and other data remains unchanged.</t>
-  </si>
-  <si>
-    <t>Test the scenario where new forecast rates are added for combinations of store group + store_group1 + store_group2 + year_month.
-Validate that the new data is correctly added to the target table without affecting existing data.
-Ensure that no duplicates are created and only relevant new data is added.</t>
-  </si>
-  <si>
     <t>Incremental Load</t>
   </si>
   <si>
@@ -312,12 +302,6 @@
   </si>
   <si>
     <t xml:space="preserve"> If an error occurs during the incremental update process, the data is rolled back to its previous state without any corruption or loss, maintaining data integrity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Updated forecast rates are correctly reflected in the target table for the specified combinations, ensuring data accuracy and consistency.</t>
-  </si>
-  <si>
-    <t>New forecast rates are successfully added to the target table without affecting existing data, ensuring data integrity and avoiding duplication.</t>
   </si>
   <si>
     <t>Source files adhere to the specified naming convention consistently, ensuring easy identification and processing.</t>
@@ -800,6 +784,73 @@
   </si>
   <si>
     <t>SELECT COUNT(*) FROM forecase_cleansed WHERE FCST_RATE IS NULL AND FCST_RATE_1 IS NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify scenario when new forecast rate are ingested from the source for the already existed combination of store group + store_group1 + store_group2 + year_month.
+</t>
+  </si>
+  <si>
+    <t>Forecast rates values should be updated with new values.</t>
+  </si>
+  <si>
+    <t>Forecast Rate Update no new records</t>
+  </si>
+  <si>
+    <t>Verify that when new forecast rates are ingested from the source for the already existed combination of store group + store_group1 + store_group2 + year_month, no new records are added for this existed combination.</t>
+  </si>
+  <si>
+    <t>Only already existed record should be updated, no new records should be added for already existed store group + store_group1 + store_group2 + year_month</t>
+  </si>
+  <si>
+    <t>Verify scenario when forecast rates are ingested from the source for new combination of store group + store_group1 + store_group2 + year_month.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New records should be inserted with new combination of store group + store_group1 + store_group2 + year_month. </t>
+  </si>
+  <si>
+    <t>Updation date postive scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that value of "UpdateDateTime" was updated after forecast rates were updated for already existing combination of store group + store_group1+ store_group2 + year_month </t>
+  </si>
+  <si>
+    <t>The UpdateDateTime value for the updated records should now be greater than the date/time when the incremental load started.</t>
+  </si>
+  <si>
+    <t>Updation date negative scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that value of "UpdateDateTime" was not changed if forecast rates were not updated for already existing combination of store group + store_group1+ store_group2 + year_month </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The UpdateDateTime value for the non updated records should not be updated or changed post-incremental load.</t>
+  </si>
+  <si>
+    <t>InsertDateTime while updation logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that value of "InsertDateTime" was not updated after forecast rates were updated for already existing combination of store group + store_group1+ store_group2 + year_month </t>
+  </si>
+  <si>
+    <t>InsertDateTime value should not be changed</t>
+  </si>
+  <si>
+    <t>InsertDateTime while inserting logic</t>
+  </si>
+  <si>
+    <t>Verify that if record is inserted with new combination of group + store_group1+ store_group2 + year_month, then "InsertDateTime" value is correctly inserted.</t>
+  </si>
+  <si>
+    <t>InsertDateTime date value should equal to date of incremental load when this record was inserted.</t>
+  </si>
+  <si>
+    <t>Processing records more than one time</t>
+  </si>
+  <si>
+    <t>Verify that if the same record Is ingested as part of incremental load more then once, "UpdateDateTime" date is only updated first time.</t>
+  </si>
+  <si>
+    <t>UpdateDateTime should be updated only first time, if the same record is ingested more then once.</t>
   </si>
 </sst>
 </file>
@@ -930,7 +981,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -973,6 +1024,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1255,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCCC296-2BB6-4C22-A4E3-D35AA4A9CD78}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="81" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1267,7 +1321,7 @@
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.88671875" customWidth="1"/>
     <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="32.21875" style="6" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" customWidth="1"/>
   </cols>
@@ -1303,19 +1357,19 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1327,19 +1381,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1351,19 +1405,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1375,19 +1429,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1399,19 +1453,19 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1423,19 +1477,19 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1447,19 +1501,19 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1471,19 +1525,19 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1495,19 +1549,19 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1519,19 +1573,19 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1543,19 +1597,19 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1567,19 +1621,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1591,19 +1645,19 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1615,19 +1669,19 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1639,19 +1693,19 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1666,16 +1720,16 @@
         <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G17" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1690,16 +1744,16 @@
         <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1714,16 +1768,16 @@
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1738,16 +1792,16 @@
         <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1762,16 +1816,16 @@
         <v>33</v>
       </c>
       <c r="D21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1786,16 +1840,16 @@
         <v>33</v>
       </c>
       <c r="D22" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>29</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1810,16 +1864,16 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="72.599999999999994" x14ac:dyDescent="0.35">
@@ -1834,16 +1888,16 @@
         <v>33</v>
       </c>
       <c r="D24" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="72.599999999999994" x14ac:dyDescent="0.35">
@@ -1858,16 +1912,16 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1879,19 +1933,19 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1903,19 +1957,19 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>37</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
@@ -1927,19 +1981,19 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G28" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
@@ -1951,19 +2005,19 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -1975,216 +2029,207 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="G31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>43</v>
-      </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>223</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>42</v>
+        <v>224</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>88</v>
+        <v>225</v>
       </c>
       <c r="G32" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="G33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="D33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G33" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>228</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>45</v>
+        <v>229</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="G34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>231</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>46</v>
+        <v>232</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>234</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>47</v>
+        <v>235</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>92</v>
+        <v>236</v>
       </c>
       <c r="G36" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>237</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>48</v>
+        <v>238</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>93</v>
+        <v>239</v>
       </c>
       <c r="G37" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>49</v>
+        <v>241</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="G38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B39" t="s">
@@ -2194,21 +2239,20 @@
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B40" t="s">
@@ -2218,21 +2262,20 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="G40" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B41" t="s">
@@ -2242,21 +2285,20 @@
         <v>33</v>
       </c>
       <c r="D41" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A42">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B42" t="s">
@@ -2266,21 +2308,20 @@
         <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G42" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B43" t="s">
@@ -2290,64 +2331,200 @@
         <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G45" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" t="s">
+        <v>132</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="s">
+        <v>134</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G44" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" t="s">
-        <v>162</v>
+      <c r="D50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G50" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G51" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2359,8 +2536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2413,22 +2590,22 @@
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2440,22 +2617,22 @@
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2467,22 +2644,22 @@
         <v>7</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="G4" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2494,22 +2671,22 @@
         <v>7</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>150</v>
-      </c>
       <c r="G5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2521,22 +2698,22 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2548,22 +2725,22 @@
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" t="s">
         <v>157</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I7" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2575,22 +2752,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2602,22 +2779,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E9" t="s">
         <v>153</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" t="s">
         <v>157</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="I9" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2629,22 +2806,22 @@
         <v>7</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" t="s">
         <v>157</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="I10" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2656,22 +2833,22 @@
         <v>7</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="G11" t="s">
-        <v>161</v>
-      </c>
       <c r="I11" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2683,25 +2860,25 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G12" t="s">
         <v>157</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="G12" t="s">
-        <v>161</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2713,25 +2890,25 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G13" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2743,25 +2920,25 @@
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G14" t="s">
-        <v>161</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>168</v>
-      </c>
       <c r="I14" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2773,25 +2950,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="G15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2803,25 +2980,25 @@
         <v>7</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -2833,25 +3010,25 @@
         <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -2863,25 +3040,25 @@
         <v>7</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" t="s">
+        <v>160</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E18" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="G18" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
@@ -2893,25 +3070,25 @@
         <v>7</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
+        <v>159</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2923,25 +3100,25 @@
         <v>7</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H20" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2953,25 +3130,25 @@
         <v>7</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H21" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -2983,25 +3160,25 @@
         <v>7</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H22" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -3013,25 +3190,25 @@
         <v>7</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="G23" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -3043,25 +3220,25 @@
         <v>7</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -3073,25 +3250,25 @@
         <v>7</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -3103,25 +3280,25 @@
         <v>7</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -3133,25 +3310,25 @@
         <v>7</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -3163,25 +3340,25 @@
         <v>7</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
@@ -3193,25 +3370,25 @@
         <v>7</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
@@ -3223,25 +3400,25 @@
         <v>7</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
@@ -3253,25 +3430,25 @@
         <v>7</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
@@ -3283,25 +3460,25 @@
         <v>7</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="69" x14ac:dyDescent="0.3">
@@ -3313,25 +3490,25 @@
         <v>7</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
@@ -3343,25 +3520,25 @@
         <v>7</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
@@ -3373,25 +3550,25 @@
         <v>7</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
@@ -3403,25 +3580,25 @@
         <v>7</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>